<commit_message>
Set ending dates for kompostori. Remove unique kohde id requirement from KompostorinKohteet
- Remove unique constraint from KompostorinKohteet for Kohde_id.
- Update required headers.
- Read all kompostoija information for better kohdennus. Read all the data to kompostoija, instead of just the prt of the building.
- Added more accurate kohdennus for kompostoijat (KompostorinKohteet).
- Split finding kohde/kohteet into two sepparate functions.
- Added check for required headers. And store failed validations.
- Updated combining ilmoitus rows to match the new requirements.
- Updated model and models to match the new requirements.
- Added second test data file, to test setting ending dates and adding KompostorinKohde to an existing Kompostori.
</commit_message>
<xml_diff>
--- a/tests/data/test_kompostori/ilmoitukset_lisaa_komposti_osakas.xlsx
+++ b/tests/data/test_kompostori/ilmoitukset_lisaa_komposti_osakas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -323,6 +323,81 @@
   </si>
   <si>
     <t xml:space="preserve">Kimppa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.1.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Käsitelty kirjaamossa (tämän kohdan täyttää käsittelijä)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muutos aikaisemman ilmoituksen tietoihin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tytti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuntematon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0400123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tytti@laulumuisto.fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hatustaheitettykatu 5B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASUNTO OY KAHDEN LAULUMUISTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HARJUKATU 44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456789A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerrostalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tammikuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helmikuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maaliskuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huhtikuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toukokuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syyskuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokakuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marraskuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joulukuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompostoria käyttää yksi rakennus, joka on ilmoitettu yllä Kompostorin sijainti -kohdassa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yksittäinen</t>
   </si>
 </sst>
 </file>
@@ -334,7 +409,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -361,6 +436,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -417,7 +506,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -451,6 +540,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -578,10 +675,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT2"/>
+  <dimension ref="A1:BT3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AZ5" activeCellId="0" sqref="AZ5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BR3" activeCellId="0" sqref="BR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -963,7 +1060,174 @@
         <v>100</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BB3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BQ3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BR3" s="8" t="n">
+        <v>46446</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" display="tytti@laulumuisto.fi"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>